<commit_message>
Updated Companies.xlsx with new company list
</commit_message>
<xml_diff>
--- a/Companies.xlsx
+++ b/Companies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88fd548838687380/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88fd548838687380/Desktop/Portfolio Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{3F0B3112-86D7-4EBF-904D-642080482AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEFEFFC5-7CF8-4E3D-A325-A01555880B88}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{3F0B3112-86D7-4EBF-904D-642080482AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F014046-FAA6-4B43-8E8A-564F356023E8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D5AB9FC5-6068-4EFD-AB2E-8AF9EED9D511}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="278">
   <si>
     <t>AAPL</t>
   </si>
@@ -594,6 +594,282 @@
   </si>
   <si>
     <t>Risk-Free Rate</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>NSRGY</t>
+  </si>
+  <si>
+    <t>SNY</t>
+  </si>
+  <si>
+    <t>ORLY</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>MELI</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>INTU</t>
+  </si>
+  <si>
+    <t>DELL</t>
+  </si>
+  <si>
+    <t>PYPL</t>
+  </si>
+  <si>
+    <t>ABNB</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>EXC</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>EQIX</t>
+  </si>
+  <si>
+    <t>ILMN</t>
+  </si>
+  <si>
+    <t>PLTR</t>
+  </si>
+  <si>
+    <t>WDAY</t>
+  </si>
+  <si>
+    <t>TWTR</t>
+  </si>
+  <si>
+    <t>SNOW</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>DOCU</t>
+  </si>
+  <si>
+    <t>ROST</t>
+  </si>
+  <si>
+    <t>VZ</t>
+  </si>
+  <si>
+    <t>DLR</t>
+  </si>
+  <si>
+    <t>HCA</t>
+  </si>
+  <si>
+    <t>FISV</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>ECL</t>
+  </si>
+  <si>
+    <t>LHX</t>
+  </si>
+  <si>
+    <t>CTSH</t>
+  </si>
+  <si>
+    <t>CCI</t>
+  </si>
+  <si>
+    <t>FTNT</t>
+  </si>
+  <si>
+    <t>NOC</t>
+  </si>
+  <si>
+    <t>WBA</t>
+  </si>
+  <si>
+    <t>DHR</t>
+  </si>
+  <si>
+    <t>TROW</t>
+  </si>
+  <si>
+    <t>ALGN</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>NEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toyota Motor Corporation  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP SE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alibaba Group  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nestlé  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanofi  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O'Reilly Automotive  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Parcel Service  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVS Health  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic Data Processing  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citigroup  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MercadoLibre  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ford Motor Company  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intuit  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dell Technologies  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PayPal Holdings  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airbnb  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank of New York Mellon  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exelon Corporation  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micron Technology  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equinix  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intuitive Surgical  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palantir Technologies  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workday  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twitter (X)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snowflake Inc.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoom Video Communications  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DocuSign  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross Stores  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verizon Communications  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Realty Trust  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCA Healthcare  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiserv  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marriott International  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecolab  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sherwin-Williams  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3Harris Technologies  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognizant Technology Solutions  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crown Castle International  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortinet  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northrop Grumman  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walgreens Boots Alliance  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danaher Corporation  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T. Rowe Price Group  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Align Technology  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Mills  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newmont Corporation </t>
   </si>
 </sst>
 </file>
@@ -646,6 +922,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -965,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1395AD-A8C5-4BCF-8A25-C743F243FD5D}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1739,6 +2019,376 @@
         <v>184</v>
       </c>
     </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>187</v>
+      </c>
+      <c r="B97" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>190</v>
+      </c>
+      <c r="B100" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>191</v>
+      </c>
+      <c r="B101" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>192</v>
+      </c>
+      <c r="B102" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B103" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>194</v>
+      </c>
+      <c r="B104" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>196</v>
+      </c>
+      <c r="B106" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>197</v>
+      </c>
+      <c r="B107" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>198</v>
+      </c>
+      <c r="B108" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>199</v>
+      </c>
+      <c r="B109" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>200</v>
+      </c>
+      <c r="B110" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>201</v>
+      </c>
+      <c r="B111" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>202</v>
+      </c>
+      <c r="B112" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>203</v>
+      </c>
+      <c r="B113" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>204</v>
+      </c>
+      <c r="B114" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>205</v>
+      </c>
+      <c r="B115" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>206</v>
+      </c>
+      <c r="B116" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>208</v>
+      </c>
+      <c r="B118" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>209</v>
+      </c>
+      <c r="B119" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>210</v>
+      </c>
+      <c r="B120" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>211</v>
+      </c>
+      <c r="B121" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>212</v>
+      </c>
+      <c r="B122" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>213</v>
+      </c>
+      <c r="B123" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>214</v>
+      </c>
+      <c r="B124" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>215</v>
+      </c>
+      <c r="B125" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>216</v>
+      </c>
+      <c r="B126" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>217</v>
+      </c>
+      <c r="B127" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>218</v>
+      </c>
+      <c r="B128" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>219</v>
+      </c>
+      <c r="B129" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>220</v>
+      </c>
+      <c r="B130" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>221</v>
+      </c>
+      <c r="B131" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>222</v>
+      </c>
+      <c r="B132" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>223</v>
+      </c>
+      <c r="B133" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>224</v>
+      </c>
+      <c r="B134" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>225</v>
+      </c>
+      <c r="B135" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>226</v>
+      </c>
+      <c r="B136" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>227</v>
+      </c>
+      <c r="B137" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>228</v>
+      </c>
+      <c r="B138" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>229</v>
+      </c>
+      <c r="B139" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>230</v>
+      </c>
+      <c r="B140" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B141" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B142" t="s">
+        <v>277</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>